<commit_message>
retrain and predict with SVC model
</commit_message>
<xml_diff>
--- a/chi13/moveek.xlsx
+++ b/chi13/moveek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macos/film-comment-sentiment-classification/chi13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{941C0315-D74F-1C4A-8653-1D1370CE1DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354BEB82-4427-F144-8663-DE1E97BEAAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{B33819AB-1E35-A048-BEC7-8CFB599E2F90}"/>
   </bookViews>
@@ -454,12 +454,12 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.5" customWidth="1"/>
+    <col min="1" max="1" width="210.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -542,7 +542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="180" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>